<commit_message>
UI form input employee
</commit_message>
<xml_diff>
--- a/public/discipline-assesment/discipline-assesment (2).xlsx
+++ b/public/discipline-assesment/discipline-assesment (2).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10940E4E-B6B9-BA4B-ACF4-96F9655E5679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628B0F42-4F39-8D43-BD81-AFABDEF88723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="14920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -48,10 +48,10 @@
     <t>Terlambat</t>
   </si>
   <si>
-    <t>EN-4-095</t>
+    <t>EN-4-025</t>
   </si>
   <si>
-    <t>Rahmat Hidayat</t>
+    <t>Ade Nurjaya</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
approval SP, notif heaeder dll
</commit_message>
<xml_diff>
--- a/public/discipline-assesment/discipline-assesment (2).xlsx
+++ b/public/discipline-assesment/discipline-assesment (2).xlsx
@@ -8,15 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628B0F42-4F39-8D43-BD81-AFABDEF88723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6C22F5-BF02-F54C-87C0-725F45946B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="14920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -48,10 +56,10 @@
     <t>Terlambat</t>
   </si>
   <si>
-    <t>EN-4-025</t>
+    <t>EN-4-095</t>
   </si>
   <si>
-    <t>Ade Nurjaya</t>
+    <t>Rahmat Hidayat</t>
   </si>
 </sst>
 </file>
@@ -70,14 +78,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -539,7 +547,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -574,7 +582,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4">
         <v>2024</v>
@@ -597,7 +605,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4">
         <v>2024</v>
@@ -618,7 +626,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4" s="4">
         <v>2024</v>
@@ -639,7 +647,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B5" s="4">
         <v>2024</v>
@@ -660,7 +668,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4">
         <v>2024</v>
@@ -681,7 +689,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B7" s="4">
         <v>2024</v>

</xml_diff>